<commit_message>
fix buffer and loot
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/neutralA.xlsx
+++ b/gu_in/Map.edf/neutralA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project RF X\Parser_Public_Releases\Parser_1.0.2\database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C5B38-8A83-4DC6-9557-6B688B44A5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EF85E3-1D7F-479A-B8B4-A3EA7E35208A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -7143,7 +7143,7 @@
   <dimension ref="A1:J1064"/>
   <sheetViews>
     <sheetView topLeftCell="A891" workbookViewId="0">
-      <selection activeCell="A907" sqref="A907:XFD908"/>
+      <selection activeCell="L907" sqref="L907"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39279,8 +39279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="N112" sqref="N112"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43067,8 +43067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H224"/>
   <sheetViews>
-    <sheetView topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="A205" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47319,13 +47319,13 @@
         <v>331</v>
       </c>
       <c r="C164" s="1">
-        <v>-7561</v>
+        <v>-6586</v>
       </c>
       <c r="D164" s="1">
-        <v>1042</v>
+        <v>1035</v>
       </c>
       <c r="E164" s="1">
-        <v>-5409</v>
+        <v>-5484</v>
       </c>
       <c r="F164" s="1">
         <v>20</v>
@@ -47345,13 +47345,13 @@
         <v>0</v>
       </c>
       <c r="C165" s="1">
-        <v>-7625</v>
+        <v>-6586</v>
       </c>
       <c r="D165" s="1">
-        <v>1050</v>
+        <v>1035</v>
       </c>
       <c r="E165" s="1">
-        <v>-5409</v>
+        <v>-5484</v>
       </c>
       <c r="F165" s="1">
         <v>80</v>
@@ -48694,16 +48694,16 @@
         <v>1350</v>
       </c>
       <c r="B217" s="1">
-        <v>360</v>
+        <v>300</v>
       </c>
       <c r="C217" s="1">
-        <v>-7643</v>
+        <v>-7561</v>
       </c>
       <c r="D217" s="1">
-        <v>1035</v>
+        <v>1042</v>
       </c>
       <c r="E217" s="1">
-        <v>-4523</v>
+        <v>-5409</v>
       </c>
       <c r="F217" s="1">
         <v>20</v>
@@ -48720,16 +48720,16 @@
         <v>1351</v>
       </c>
       <c r="B218" s="1">
-        <v>359</v>
+        <v>300</v>
       </c>
       <c r="C218" s="1">
-        <v>-7642</v>
+        <v>-7561</v>
       </c>
       <c r="D218" s="1">
-        <v>1035</v>
+        <v>1042</v>
       </c>
       <c r="E218" s="1">
-        <v>-4522</v>
+        <v>-5409</v>
       </c>
       <c r="F218" s="1">
         <v>20</v>
@@ -48906,7 +48906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
armor + item starting NPC & map
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/neutralA.xlsx
+++ b/gu_in/Map.edf/neutralA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\emay.dev\Parser_1.0.2\Database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3EAC4F-1E23-4C18-963A-443CABD733B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEE6394-4115-42A7-BFF5-780CE05C9BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43078,8 +43078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43615,7 +43615,7 @@
         <v>-7287</v>
       </c>
       <c r="D21" s="1">
-        <v>1037</v>
+        <v>2001037</v>
       </c>
       <c r="E21" s="1">
         <v>-6574</v>
@@ -43641,7 +43641,7 @@
         <v>-7293</v>
       </c>
       <c r="D22" s="1">
-        <v>1036</v>
+        <v>2001036</v>
       </c>
       <c r="E22" s="1">
         <v>-6487</v>
@@ -46400,7 +46400,7 @@
         <v>1040</v>
       </c>
       <c r="E128" s="1">
-        <v>-5120</v>
+        <v>-2005120</v>
       </c>
       <c r="F128" s="1">
         <v>20</v>
@@ -46426,7 +46426,7 @@
         <v>1035</v>
       </c>
       <c r="E129" s="1">
-        <v>-5071</v>
+        <v>-2005071</v>
       </c>
       <c r="F129" s="1">
         <v>200</v>
@@ -46501,7 +46501,7 @@
         <v>-7798</v>
       </c>
       <c r="D132" s="1">
-        <v>1044</v>
+        <v>2001044</v>
       </c>
       <c r="E132" s="1">
         <v>-4468</v>
@@ -46527,7 +46527,7 @@
         <v>-7705</v>
       </c>
       <c r="D133" s="1">
-        <v>1037</v>
+        <v>2001037</v>
       </c>
       <c r="E133" s="1">
         <v>-4531</v>
@@ -46553,7 +46553,7 @@
         <v>-7680</v>
       </c>
       <c r="D134" s="1">
-        <v>1041</v>
+        <v>2001041</v>
       </c>
       <c r="E134" s="1">
         <v>-4424</v>
@@ -46579,7 +46579,7 @@
         <v>-7705</v>
       </c>
       <c r="D135" s="1">
-        <v>1035</v>
+        <v>2001035</v>
       </c>
       <c r="E135" s="1">
         <v>-4528</v>
@@ -47385,7 +47385,7 @@
         <v>-9058</v>
       </c>
       <c r="D166" s="1">
-        <v>1125</v>
+        <v>2001125</v>
       </c>
       <c r="E166" s="1">
         <v>-5482</v>
@@ -47411,7 +47411,7 @@
         <v>-9058</v>
       </c>
       <c r="D167" s="1">
-        <v>1124</v>
+        <v>2001124</v>
       </c>
       <c r="E167" s="1">
         <v>-5482</v>

</xml_diff>

<commit_message>
reloc HQ buffer , Premium Shop
</commit_message>
<xml_diff>
--- a/gu_in/Map.edf/neutralA.xlsx
+++ b/gu_in/Map.edf/neutralA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\emay.dev\Parser_1.0.2\Database\gu_in\Map.edf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB89F96-1F98-45FE-BA69-9FC681532284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009BC666-7EE0-40A8-B877-97F071335D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="0" windowWidth="18480" windowHeight="11205" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5415" yWindow="0" windowWidth="18480" windowHeight="11205" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -48922,13 +48922,13 @@
         <v>356</v>
       </c>
       <c r="C225" s="1">
-        <v>-7709</v>
+        <v>-7549</v>
       </c>
       <c r="D225" s="1">
         <v>1035</v>
       </c>
       <c r="E225" s="1">
-        <v>-5339</v>
+        <v>-5373</v>
       </c>
       <c r="F225" s="1">
         <v>20</v>
@@ -48948,13 +48948,13 @@
         <v>355</v>
       </c>
       <c r="C226" s="1">
-        <v>-7709</v>
+        <v>-7549</v>
       </c>
       <c r="D226" s="1">
         <v>1035</v>
       </c>
       <c r="E226" s="1">
-        <v>-5339</v>
+        <v>-5373</v>
       </c>
       <c r="F226" s="1">
         <v>20</v>

</xml_diff>